<commit_message>
second half of project
</commit_message>
<xml_diff>
--- a/statsStuff.xlsx
+++ b/statsStuff.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanrael/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanrael/Documents/pythonProjects/statsProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F74394-A66D-B543-BD22-EF7860DEBDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29FE0DD-FE4A-234F-9493-8A6A70142EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="440" yWindow="2000" windowWidth="30240" windowHeight="17640" xr2:uid="{38EEA979-E340-6944-9CBA-282939A52CFB}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="30240" windowHeight="17640" activeTab="1" xr2:uid="{38EEA979-E340-6944-9CBA-282939A52CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="stockPrices" sheetId="1" r:id="rId1"/>
@@ -45,9 +45,6 @@
     <t>Time interval</t>
   </si>
   <si>
-    <t>Time Interval (in seconds)</t>
-  </si>
-  <si>
     <t>Stock Number</t>
   </si>
   <si>
@@ -652,6 +649,9 @@
   </si>
   <si>
     <t>12:49:49 P.M</t>
+  </si>
+  <si>
+    <t>Time Interval Seconds</t>
   </si>
 </sst>
 </file>
@@ -715,10 +715,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1040,7 +1036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A69FC81-1881-8140-8E9D-CCA8E4E05E91}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1051,15 +1047,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>415.28</v>
@@ -1067,7 +1063,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>173.23</v>
@@ -1075,7 +1071,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>919.13</v>
@@ -1083,7 +1079,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>175.39</v>
@@ -1091,7 +1087,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>139.62</v>
@@ -1099,7 +1095,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>499.75</v>
@@ -1107,7 +1103,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8">
         <v>404.98</v>
@@ -1115,7 +1111,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>754.95</v>
@@ -1123,7 +1119,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>1291.8800000000001</v>
@@ -1131,7 +1127,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>283.92</v>
@@ -1139,7 +1135,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>177.54</v>
@@ -1147,7 +1143,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>189.84</v>
@@ -1155,7 +1151,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>61.41</v>
@@ -1163,7 +1159,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15">
         <v>489.35</v>
@@ -1171,7 +1167,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>472.87</v>
@@ -1179,7 +1175,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17">
         <v>108.32</v>
@@ -1187,7 +1183,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18">
         <v>162.74</v>
@@ -1195,7 +1191,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19">
         <v>161.93</v>
@@ -1203,7 +1199,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>374.54</v>
@@ -1211,7 +1207,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>180.92</v>
@@ -1219,7 +1215,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22">
         <v>202.76</v>
@@ -1227,7 +1223,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>736.88</v>
@@ -1235,7 +1231,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24">
         <v>127.54</v>
@@ -1243,7 +1239,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25">
         <v>122.66</v>
@@ -1251,7 +1247,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B26">
         <v>306.62</v>
@@ -1259,7 +1255,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27">
         <v>35.96</v>
@@ -1267,7 +1263,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>151.88999999999999</v>
@@ -1275,7 +1271,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29">
         <v>611.08000000000004</v>
@@ -1283,7 +1279,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30">
         <v>60.5</v>
@@ -1291,7 +1287,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B31">
         <v>579.14</v>
@@ -1299,7 +1295,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32">
         <v>1.39</v>
@@ -1307,7 +1303,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33">
         <v>597.25</v>
@@ -1315,7 +1311,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>164.54</v>
@@ -1323,7 +1319,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35">
         <v>471.47</v>
@@ -1331,7 +1327,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B36">
         <v>294.31</v>
@@ -1339,7 +1335,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>120.76</v>
@@ -1347,7 +1343,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>112.46</v>
@@ -1355,7 +1351,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39">
         <v>57.61</v>
@@ -1363,7 +1359,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40">
         <v>50.07</v>
@@ -1371,7 +1367,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <v>163.68</v>
@@ -1379,7 +1375,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42">
         <v>173.08</v>
@@ -1387,7 +1383,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>45.24</v>
@@ -1395,7 +1391,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B44">
         <v>253.1</v>
@@ -1403,7 +1399,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B45">
         <v>662.64</v>
@@ -1411,7 +1407,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B46">
         <v>167.46</v>
@@ -1419,7 +1415,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B47">
         <v>197.78</v>
@@ -1427,7 +1423,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B48">
         <v>43.18</v>
@@ -1435,7 +1431,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49">
         <v>204.94</v>
@@ -1443,7 +1439,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50">
         <v>40.130000000000003</v>
@@ -1451,7 +1447,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>337.24</v>
@@ -1459,7 +1455,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>78.319999999999993</v>
@@ -1467,7 +1463,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53">
         <v>222.65</v>
@@ -1475,7 +1471,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54">
         <v>174.8</v>
@@ -1483,7 +1479,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B55">
         <v>28.01</v>
@@ -1491,7 +1487,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56">
         <v>789.56</v>
@@ -1499,7 +1495,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57">
         <v>251.18</v>
@@ -1507,7 +1503,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58">
         <v>123.68</v>
@@ -1515,7 +1511,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B59">
         <v>100.18</v>
@@ -1523,7 +1519,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B60">
         <v>276.54000000000002</v>
@@ -1531,7 +1527,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B61">
         <v>94.67</v>
@@ -1539,7 +1535,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B62">
         <v>171.82</v>
@@ -1547,7 +1543,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63">
         <v>243.26</v>
@@ -1555,7 +1551,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64">
         <v>115.02</v>
@@ -1563,7 +1559,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65">
         <v>358.39</v>
@@ -1571,7 +1567,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66">
         <v>389.4</v>
@@ -1579,7 +1575,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67">
         <v>428.61</v>
@@ -1587,7 +1583,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B68">
         <v>157.38</v>
@@ -1595,7 +1591,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B69">
         <v>199.13</v>
@@ -1603,7 +1599,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B70">
         <v>388.18</v>
@@ -1611,7 +1607,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71">
         <v>134.57</v>
@@ -1619,7 +1615,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72">
         <v>17.2</v>
@@ -1627,7 +1623,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73">
         <v>829.59</v>
@@ -1635,7 +1631,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74">
         <v>66.5</v>
@@ -1643,7 +1639,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75">
         <v>950.83</v>
@@ -1651,7 +1647,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76">
         <v>89.95</v>
@@ -1659,7 +1655,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B77">
         <v>3500</v>
@@ -1667,7 +1663,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B78">
         <v>57.15</v>
@@ -1675,7 +1671,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B79">
         <v>505.57</v>
@@ -1683,7 +1679,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B80">
         <v>184.24</v>
@@ -1691,7 +1687,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81">
         <v>297.74</v>
@@ -1699,7 +1695,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B82">
         <v>198.94</v>
@@ -1707,7 +1703,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B83">
         <v>85.74</v>
@@ -1715,7 +1711,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84">
         <v>97.22</v>
@@ -1723,7 +1719,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85">
         <v>54.4</v>
@@ -1731,7 +1727,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86">
         <v>57.45</v>
@@ -1739,7 +1735,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87">
         <v>412.45</v>
@@ -1747,7 +1743,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88">
         <v>970.57</v>
@@ -1755,7 +1751,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89">
         <v>166.67</v>
@@ -1763,7 +1759,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90">
         <v>434.91</v>
@@ -1771,7 +1767,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91">
         <v>372.65</v>
@@ -1779,7 +1775,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92">
         <v>97.42</v>
@@ -1787,7 +1783,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93">
         <v>92.4</v>
@@ -1795,7 +1791,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94">
         <v>257.75</v>
@@ -1803,7 +1799,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B95">
         <v>207.35</v>
@@ -1811,7 +1807,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96">
         <v>343.94</v>
@@ -1819,7 +1815,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97">
         <v>244.67</v>
@@ -1827,7 +1823,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98">
         <v>199.2</v>
@@ -1835,7 +1831,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99">
         <v>71.739999999999995</v>
@@ -1843,7 +1839,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100">
         <v>67.489999999999995</v>
@@ -1851,7 +1847,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101">
         <v>204.18</v>
@@ -1866,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FC9DC0-E7DC-E246-B3BC-54ED890AA89D}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1884,12 +1880,12 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="2">
         <v>4.5138888888888887E-4</v>
@@ -1900,7 +1896,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="2">
         <v>7.0601851851851847E-4</v>
@@ -1911,7 +1907,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" s="2">
         <v>4.6296296296296294E-5</v>
@@ -1922,7 +1918,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" s="2">
         <v>1.8518518518518518E-4</v>
@@ -1933,7 +1929,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="2">
         <v>4.6296296296296298E-4</v>
@@ -1944,7 +1940,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" s="2">
         <v>1.7361111111111112E-4</v>
@@ -1955,7 +1951,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" s="2">
         <v>2.199074074074074E-4</v>
@@ -1966,7 +1962,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B9" s="2">
         <v>5.7870370370370373E-5</v>
@@ -1977,7 +1973,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="2">
         <v>1.6203703703703703E-4</v>
@@ -1988,7 +1984,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="2">
         <v>6.9444444444444444E-5</v>
@@ -1999,7 +1995,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" s="2">
         <v>1.6203703703703703E-4</v>
@@ -2010,7 +2006,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2">
         <v>1.5046296296296297E-4</v>
@@ -2021,7 +2017,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B14" s="2">
         <v>1.7361111111111112E-4</v>
@@ -2032,7 +2028,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" s="2">
         <v>3.2407407407407406E-4</v>
@@ -2043,7 +2039,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B16" s="2">
         <v>6.9444444444444444E-5</v>
@@ -2054,7 +2050,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B17" s="2">
         <v>4.3981481481481481E-4</v>
@@ -2065,7 +2061,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18" s="2">
         <v>8.3333333333333339E-4</v>
@@ -2076,7 +2072,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" s="2">
         <v>1.273148148148148E-4</v>
@@ -2087,7 +2083,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B20" s="2">
         <v>2.3148148148148149E-4</v>
@@ -2098,7 +2094,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" s="2">
         <v>8.1018518518518516E-5</v>
@@ -2109,7 +2105,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B22" s="2">
         <v>1.9675925925925926E-4</v>
@@ -2120,7 +2116,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B23" s="2">
         <v>1.1574074074074075E-4</v>
@@ -2131,7 +2127,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B24" s="2">
         <v>1.5046296296296297E-4</v>
@@ -2142,7 +2138,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B25" s="2">
         <v>1.273148148148148E-4</v>
@@ -2153,7 +2149,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B26" s="4">
         <v>7.407407407407407E-4</v>
@@ -2164,7 +2160,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B27" s="4">
         <v>4.1666666666666669E-4</v>
@@ -2175,7 +2171,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B28" s="4">
         <v>1.1574074074074075E-4</v>
@@ -2186,7 +2182,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B29" s="4">
         <v>9.2592592592592588E-5</v>
@@ -2197,7 +2193,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B30" s="4">
         <v>2.4305555555555555E-4</v>
@@ -2208,7 +2204,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B31" s="4">
         <v>2.3148148148148147E-5</v>
@@ -2219,7 +2215,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B32" s="2">
         <v>2.6620370370370372E-4</v>
@@ -2230,7 +2226,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B33" s="2">
         <v>3.5879629629629629E-4</v>
@@ -2241,7 +2237,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B34" s="2">
         <v>1.9675925925925926E-4</v>
@@ -2252,7 +2248,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B35" s="2">
         <v>1.7361111111111112E-4</v>
@@ -2263,7 +2259,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B36" s="4">
         <v>9.2592592592592588E-5</v>
@@ -2274,7 +2270,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B37" s="4">
         <v>9.6064814814814819E-4</v>
@@ -2285,7 +2281,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B38" s="4">
         <v>7.0601851851851847E-4</v>
@@ -2296,7 +2292,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B39" s="4">
         <v>1.1574074074074075E-4</v>
@@ -2307,7 +2303,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B40" s="4">
         <v>2.6620370370370372E-4</v>
@@ -2318,7 +2314,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B41" s="4">
         <v>1.5046296296296297E-4</v>
@@ -2329,7 +2325,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B42" s="2">
         <v>8.1018518518518516E-5</v>
@@ -2340,7 +2336,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B43" s="2">
         <v>5.6712962962962967E-4</v>
@@ -2351,7 +2347,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B44" s="2">
         <v>6.9444444444444444E-5</v>
@@ -2362,7 +2358,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B45" s="2">
         <v>1.1574074074074073E-3</v>
@@ -2373,7 +2369,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B46" s="4">
         <v>2.3148148148148147E-5</v>
@@ -2384,7 +2380,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B47" s="4">
         <v>2.6620370370370372E-4</v>
@@ -2395,7 +2391,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B48" s="4">
         <v>1.7361111111111112E-4</v>
@@ -2406,7 +2402,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B49" s="4">
         <v>7.8703703703703705E-4</v>
@@ -2417,7 +2413,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B50" s="4">
         <v>1.1574074074074075E-4</v>
@@ -2428,7 +2424,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B51" s="4">
         <v>2.0833333333333335E-4</v>
@@ -2439,7 +2435,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B52" s="2">
         <v>8.1018518518518516E-5</v>
@@ -2450,7 +2446,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B53" s="2">
         <v>1.9675925925925926E-4</v>
@@ -2461,7 +2457,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B54" s="2">
         <v>3.9351851851851852E-4</v>
@@ -2472,7 +2468,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B55" s="2">
         <v>3.1250000000000001E-4</v>
@@ -2483,7 +2479,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B56" s="4">
         <v>2.8935185185185184E-4</v>
@@ -2494,7 +2490,7 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B57" s="4">
         <v>1.0185185185185184E-3</v>
@@ -2505,7 +2501,7 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B58" s="4">
         <v>8.1018518518518516E-5</v>
@@ -2516,7 +2512,7 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B59" s="4">
         <v>6.4814814814814813E-4</v>
@@ -2527,7 +2523,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B60" s="4">
         <v>9.837962962962962E-4</v>
@@ -2538,7 +2534,7 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B61" s="4">
         <v>5.7870370370370367E-4</v>
@@ -2549,7 +2545,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B62" s="2">
         <v>3.4722222222222222E-5</v>
@@ -2560,7 +2556,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B63" s="2">
         <v>4.1666666666666669E-4</v>
@@ -2571,7 +2567,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B64" s="2">
         <v>2.3148148148148147E-5</v>
@@ -2582,7 +2578,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B65" s="2">
         <v>6.7129629629629625E-4</v>
@@ -2593,7 +2589,7 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B66" s="4">
         <v>1.0879629629629629E-3</v>
@@ -2604,7 +2600,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B67" s="4">
         <v>6.3657407407407413E-4</v>
@@ -2615,7 +2611,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B68" s="4">
         <v>2.3148148148148149E-4</v>
@@ -2626,7 +2622,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B69" s="4">
         <v>7.291666666666667E-4</v>
@@ -2637,7 +2633,7 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B70" s="4">
         <v>4.5138888888888887E-4</v>
@@ -2649,7 +2645,7 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B71" s="4">
         <v>0.12503472222222223</v>
@@ -2660,7 +2656,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B72" s="2">
         <v>6.9444444444444444E-5</v>
@@ -2671,7 +2667,7 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B73" s="2">
         <v>3.4722222222222222E-5</v>
@@ -2682,7 +2678,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B74" s="2">
         <v>1.5046296296296297E-4</v>
@@ -2693,7 +2689,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B75" s="2">
         <v>8.6805555555555551E-4</v>
@@ -2704,7 +2700,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B76" s="4">
         <v>2.3148148148148147E-5</v>
@@ -2715,7 +2711,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B77" s="4">
         <v>4.0509259259259258E-4</v>
@@ -2726,7 +2722,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B78" s="4">
         <v>6.9444444444444444E-5</v>
@@ -2737,7 +2733,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B79" s="4">
         <v>1.7361111111111112E-4</v>
@@ -2748,7 +2744,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B80" s="4">
         <v>1.4236111111111112E-3</v>
@@ -2759,7 +2755,7 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B81" s="4">
         <v>1.5046296296296297E-4</v>
@@ -2770,7 +2766,7 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B82" s="2">
         <v>4.6296296296296294E-5</v>
@@ -2781,7 +2777,7 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B83" s="2">
         <v>1.8518518518518518E-4</v>
@@ -2792,7 +2788,7 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B84" s="2">
         <v>2.3148148148148147E-5</v>
@@ -2803,7 +2799,7 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B85" s="2">
         <v>2.6620370370370372E-4</v>
@@ -2814,7 +2810,7 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B86" s="2">
         <v>4.7453703703703704E-4</v>
@@ -2825,7 +2821,7 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B87" s="2">
         <v>3.4722222222222224E-4</v>
@@ -2836,7 +2832,7 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B88" s="2">
         <v>1.6203703703703703E-4</v>
@@ -2847,7 +2843,7 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B89" s="2">
         <v>9.2592592592592588E-5</v>
@@ -2858,7 +2854,7 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B90" s="2">
         <v>7.0601851851851847E-4</v>
@@ -2869,7 +2865,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B91" s="2">
         <v>1.261574074074074E-3</v>
@@ -2880,7 +2876,7 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B92" s="2">
         <v>2.0833333333333335E-4</v>
@@ -2891,7 +2887,7 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B93" s="2">
         <v>1.6203703703703703E-4</v>
@@ -2902,7 +2898,7 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B94" s="2">
         <v>4.861111111111111E-4</v>
@@ -2913,7 +2909,7 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B95" s="2">
         <v>9.2592592592592588E-5</v>
@@ -2924,7 +2920,7 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B96" s="2">
         <v>6.9444444444444444E-5</v>
@@ -2935,7 +2931,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B97" s="2">
         <v>2.3148148148148147E-5</v>
@@ -2946,7 +2942,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B98" s="2">
         <v>3.9351851851851852E-4</v>
@@ -2957,7 +2953,7 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B99" s="2">
         <v>2.8935185185185184E-4</v>
@@ -2968,7 +2964,7 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B100" s="2">
         <v>1.273148148148148E-4</v>
@@ -2979,7 +2975,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B101" s="2">
         <v>1.6203703703703703E-4</v>

</xml_diff>